<commit_message>
fixed line in spreadsheet
</commit_message>
<xml_diff>
--- a/masks/code/TKIDModule_spreadsheet_20200520_AW_special.xlsx
+++ b/masks/code/TKIDModule_spreadsheet_20200520_AW_special.xlsx
@@ -4292,7 +4292,7 @@
         <v>4.54</v>
       </c>
       <c r="E51" s="1" t="n">
-        <v>-2.986</v>
+        <v>-2.972</v>
       </c>
       <c r="F51" s="1" t="n">
         <v>8.619999999999999</v>
@@ -4307,10 +4307,10 @@
         <v>8.85</v>
       </c>
       <c r="J51" s="1" t="n">
-        <v>-2.6</v>
+        <v>-2.586</v>
       </c>
       <c r="K51" s="1" t="n">
-        <v>-3.4</v>
+        <v>-3.386</v>
       </c>
       <c r="L51" s="1" t="n"/>
       <c r="M51" s="1" t="n">
@@ -4323,7 +4323,7 @@
         <v>4.54</v>
       </c>
       <c r="P51" s="1" t="n">
-        <v>0.9569999999999999</v>
+        <v>0.9710000000000001</v>
       </c>
       <c r="Q51" s="1" t="n"/>
       <c r="R51" s="1" t="n"/>

</xml_diff>